<commit_message>
avances para revisión 2
</commit_message>
<xml_diff>
--- a/Otros documentos/Documentación/Matriz_RACI_CatchAI.xlsx
+++ b/Otros documentos/Documentación/Matriz_RACI_CatchAI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\CatchAI\Otros documentos\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C9804C-1A2F-46F5-B7DF-CB974F6203F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7CC466E-D1C8-4171-B0E8-0DDA5F748585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,6 +55,9 @@
     <t>Pruebas internas y validación técnica</t>
   </si>
   <si>
+    <t>Validación piloto con usuarios sordos</t>
+  </si>
+  <si>
     <t>Informes de avance y minutas</t>
   </si>
   <si>
@@ -92,9 +95,6 @@
   </si>
   <si>
     <t>Canal 13C (C)</t>
-  </si>
-  <si>
-    <t>Validación piloto con usuarios especialistas</t>
   </si>
 </sst>
 </file>
@@ -181,21 +181,15 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
         <right style="thin">
           <color auto="1"/>
         </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -216,15 +210,21 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
         <right style="thin">
           <color auto="1"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -241,10 +241,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{07C50C0E-69A3-4D26-8FE3-F2E34AE1D1B7}" name="Tabla1" displayName="Tabla1" ref="A1:F14" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{07C50C0E-69A3-4D26-8FE3-F2E34AE1D1B7}" name="Tabla1" displayName="Tabla1" ref="A1:F14" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:F14" xr:uid="{07C50C0E-69A3-4D26-8FE3-F2E34AE1D1B7}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E91D2711-B208-4A96-A3FB-8C8F9B4F5DF6}" name="Actividad" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E91D2711-B208-4A96-A3FB-8C8F9B4F5DF6}" name="Actividad" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{D3D7495D-73F3-44D3-B65A-75465FE2DCE0}" name="Eyleen Collado (PM)"/>
     <tableColumn id="3" xr3:uid="{D3735137-9DD7-45ED-A384-2DE94664FD44}" name="Marcos Hernández (Dev)"/>
     <tableColumn id="4" xr3:uid="{77E5D43D-FF18-48EB-9920-8D2C80FB07F8}" name="Marcos Bombalás (SM)"/>
@@ -545,7 +545,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,22 +560,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -583,19 +583,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -603,19 +603,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -623,19 +623,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -643,19 +643,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -663,19 +663,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -683,19 +683,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -703,19 +703,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -723,19 +723,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -743,19 +743,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -763,79 +763,79 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>